<commit_message>
added a couple of new abilities and materials.
</commit_message>
<xml_diff>
--- a/Enchantments.xlsx
+++ b/Enchantments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\Git Repositories\materials_and_crafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D53F02-210D-4908-ABDF-105AA03A068B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22CC949-F259-462A-B971-4CF514E981D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="1" activeTab="4" xr2:uid="{11AE916A-0CE2-4C8E-9116-BD67A671ABA1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="1" activeTab="2" xr2:uid="{11AE916A-0CE2-4C8E-9116-BD67A671ABA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Point Buy" sheetId="4" r:id="rId1"/>
@@ -1658,9 +1658,6 @@
     </r>
   </si>
   <si>
-    <t>72 ~ 101 MCI</t>
-  </si>
-  <si>
     <t>Cast light</t>
   </si>
   <si>
@@ -1869,6 +1866,9 @@
   </si>
   <si>
     <t>*Minimum of 5 ft.</t>
+  </si>
+  <si>
+    <t>72 ~ 101 (33 ~ 62) MCI</t>
   </si>
 </sst>
 </file>
@@ -2200,142 +2200,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2359,32 +2236,155 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="13" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2707,7 +2707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E34FB7-A163-4E1A-8D89-59CF44F6A322}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -2718,31 +2718,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="95"/>
+      <c r="C1" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="95"/>
       <c r="F1" s="12" t="s">
         <v>101</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
       <c r="J1" s="21"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
       <c r="F2" t="s">
         <v>100</v>
       </c>
@@ -2754,12 +2754,12 @@
       <c r="J2" s="21"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="97" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
       <c r="F3" t="s">
         <v>102</v>
       </c>
@@ -2771,14 +2771,14 @@
       <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
-        <v>197</v>
-      </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="D4" s="46"/>
+      <c r="A4" s="59" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" s="59"/>
+      <c r="C4" s="60" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" s="60"/>
       <c r="F4" t="s">
         <v>103</v>
       </c>
@@ -2790,14 +2790,14 @@
       <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
-        <v>198</v>
-      </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="46" t="s">
-        <v>193</v>
-      </c>
-      <c r="D5" s="46"/>
+      <c r="A5" s="59" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" s="59"/>
+      <c r="C5" s="60" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" s="60"/>
       <c r="F5" t="s">
         <v>104</v>
       </c>
@@ -2809,14 +2809,14 @@
       <c r="J5" s="21"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="69" t="s">
-        <v>202</v>
-      </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="102" t="s">
-        <v>194</v>
-      </c>
-      <c r="D6" s="102"/>
+      <c r="A6" s="65" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="65"/>
+      <c r="C6" s="66" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" s="66"/>
       <c r="F6" t="s">
         <v>105</v>
       </c>
@@ -2828,73 +2828,73 @@
       <c r="J6" s="21"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="96" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="71"/>
-      <c r="C9" s="70" t="s">
+      <c r="B9" s="80"/>
+      <c r="C9" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="70"/>
+      <c r="D9" s="81"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="93" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="51" t="s">
+      <c r="B11" s="77"/>
+      <c r="C11" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="51"/>
+      <c r="D11" s="78"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="39" t="s">
+      <c r="B12" s="75"/>
+      <c r="C12" s="76" t="s">
         <v>124</v>
       </c>
-      <c r="D12" s="39"/>
+      <c r="D12" s="76"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="29" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="29" t="s">
         <v>43</v>
       </c>
       <c r="D13" s="19" t="s">
@@ -2902,13 +2902,13 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="29" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="29" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="19" t="s">
@@ -2916,121 +2916,121 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="29" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="72" t="s">
+      <c r="D15" s="94" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="29" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="44"/>
+      <c r="D16" s="69"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
+      <c r="A17" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="33" t="s">
+      <c r="B17" s="59"/>
+      <c r="C17" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="D17" s="33"/>
+      <c r="D17" s="72"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="51" t="s">
+      <c r="B19" s="84"/>
+      <c r="C19" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="54"/>
+      <c r="D19" s="85"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="58"/>
-      <c r="C20" s="53" t="s">
+      <c r="B20" s="82"/>
+      <c r="C20" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="53"/>
+      <c r="D20" s="83"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="59" t="s">
+      <c r="A22" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="59"/>
-      <c r="C22" s="63" t="s">
+      <c r="B22" s="77"/>
+      <c r="C22" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="63"/>
+      <c r="D22" s="86"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="65" t="s">
+      <c r="B23" s="88"/>
+      <c r="C23" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="65"/>
+      <c r="D23" s="90"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="64" t="s">
+      <c r="A24" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="65" t="s">
+      <c r="B24" s="88"/>
+      <c r="C24" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="65"/>
+      <c r="D24" s="90"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="s">
-        <v>203</v>
-      </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="35" t="s">
+      <c r="A25" s="69" t="s">
+        <v>202</v>
+      </c>
+      <c r="B25" s="69"/>
+      <c r="C25" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="35"/>
+      <c r="D25" s="67"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="49" t="s">
+      <c r="A26" s="69"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="30" t="s">
         <v>84</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -3038,256 +3038,256 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="49" t="s">
+      <c r="A27" s="69"/>
+      <c r="B27" s="69"/>
+      <c r="C27" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="66" t="s">
+      <c r="D27" s="91" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="45"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="49" t="s">
+      <c r="A28" s="89"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="67"/>
+      <c r="D28" s="92"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="59" t="s">
+      <c r="A30" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="B30" s="59"/>
-      <c r="C30" s="54" t="s">
+      <c r="B30" s="77"/>
+      <c r="C30" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="55"/>
+      <c r="D30" s="87"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="73" t="s">
+      <c r="A31" s="33" t="s">
         <v>99</v>
       </c>
       <c r="B31" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="F31" t="s">
         <v>205</v>
       </c>
-      <c r="C31" s="73" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="F31" t="s">
-        <v>206</v>
-      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="59" t="s">
+      <c r="A33" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="59"/>
-      <c r="C33" s="51" t="s">
+      <c r="B33" s="77"/>
+      <c r="C33" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="52"/>
+      <c r="D33" s="79"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="60" t="s">
+      <c r="A34" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="60"/>
-      <c r="C34" s="39" t="s">
+      <c r="B34" s="59"/>
+      <c r="C34" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="39"/>
+      <c r="D34" s="76"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="59" t="s">
+      <c r="A36" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="59"/>
-      <c r="C36" s="42" t="s">
+      <c r="B36" s="77"/>
+      <c r="C36" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="42"/>
+      <c r="D36" s="68"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="60" t="s">
+      <c r="A37" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="60"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="61" t="s">
+      <c r="A38" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="61"/>
-      <c r="C38" s="35" t="s">
+      <c r="B38" s="62"/>
+      <c r="C38" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="35"/>
+      <c r="D38" s="67"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="61" t="s">
+      <c r="A39" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="61"/>
-      <c r="C39" s="35" t="s">
+      <c r="B39" s="62"/>
+      <c r="C39" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="35"/>
+      <c r="D39" s="67"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="61" t="s">
+      <c r="A40" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="61"/>
-      <c r="C40" s="35" t="s">
+      <c r="B40" s="62"/>
+      <c r="C40" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="D40" s="35"/>
+      <c r="D40" s="67"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="61" t="s">
+      <c r="A42" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="B42" s="61"/>
-      <c r="C42" s="42" t="s">
+      <c r="B42" s="62"/>
+      <c r="C42" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="42"/>
+      <c r="D42" s="68"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="61" t="s">
+      <c r="A43" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="B43" s="61"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
+      <c r="B43" s="62"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="69"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="61" t="s">
+      <c r="A44" s="62" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="61"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="61" t="s">
+      <c r="A45" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="B45" s="61"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="69"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="61" t="s">
+      <c r="A46" s="62" t="s">
         <v>137</v>
       </c>
-      <c r="B46" s="61"/>
-      <c r="C46" s="36" t="s">
+      <c r="B46" s="62"/>
+      <c r="C46" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="D46" s="36"/>
+      <c r="D46" s="70"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="61" t="s">
+      <c r="A47" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="B47" s="61"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
+      <c r="B47" s="62"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="70"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="61" t="s">
+      <c r="A48" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="B48" s="61"/>
-      <c r="C48" s="35" t="s">
+      <c r="B48" s="62"/>
+      <c r="C48" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="D48" s="35"/>
+      <c r="D48" s="67"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="61" t="s">
+      <c r="A49" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="B49" s="61"/>
-      <c r="C49" s="35" t="s">
+      <c r="B49" s="62"/>
+      <c r="C49" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="D49" s="35"/>
+      <c r="D49" s="67"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="61" t="s">
+      <c r="A50" s="62" t="s">
         <v>141</v>
       </c>
-      <c r="B50" s="61"/>
-      <c r="C50" s="35" t="s">
+      <c r="B50" s="62"/>
+      <c r="C50" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="D50" s="35"/>
+      <c r="D50" s="67"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="61" t="s">
+      <c r="A51" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="B51" s="61"/>
-      <c r="C51" s="35" t="s">
+      <c r="B51" s="62"/>
+      <c r="C51" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="D51" s="35"/>
+      <c r="D51" s="67"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="43" t="s">
+      <c r="A52" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
+      <c r="B52" s="61"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="61"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="42" t="s">
+      <c r="A53" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="42"/>
-      <c r="C53" s="68" t="s">
+      <c r="B53" s="68"/>
+      <c r="C53" s="32" t="s">
         <v>88</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -3295,9 +3295,9 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="44"/>
-      <c r="B54" s="44"/>
-      <c r="C54" s="68" t="s">
+      <c r="A54" s="69"/>
+      <c r="B54" s="69"/>
+      <c r="C54" s="32" t="s">
         <v>89</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -3305,32 +3305,32 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="69" t="s">
+      <c r="A55" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="B55" s="69"/>
-      <c r="C55" s="30" t="s">
+      <c r="B55" s="65"/>
+      <c r="C55" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="D55" s="37"/>
+      <c r="D55" s="74"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="43" t="s">
-        <v>192</v>
-      </c>
-      <c r="B56" s="43"/>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
+      <c r="A56" s="61" t="s">
+        <v>191</v>
+      </c>
+      <c r="B56" s="61"/>
+      <c r="C56" s="61"/>
+      <c r="D56" s="61"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="61" t="s">
+      <c r="A57" s="62" t="s">
         <v>164</v>
       </c>
-      <c r="B57" s="61"/>
-      <c r="C57" s="92" t="s">
+      <c r="B57" s="62"/>
+      <c r="C57" s="63" t="s">
         <v>165</v>
       </c>
-      <c r="D57" s="93"/>
+      <c r="D57" s="64"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
@@ -3338,11 +3338,53 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A25:B28"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:D37"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C38:D38"/>
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="A6:B6"/>
@@ -3359,6 +3401,11 @@
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A56:D56"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="A41:D41"/>
@@ -3370,53 +3417,6 @@
     <mergeCell ref="A53:B54"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:D37"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A25:B28"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3427,8 +3427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C151C45-D523-442D-92BB-09BBD578EF45}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3438,11 +3438,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
@@ -3472,19 +3472,19 @@
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="98"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="98"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -3523,11 +3523,11 @@
       <c r="A9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
+      <c r="B10" s="95"/>
+      <c r="C10" s="95"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -3555,10 +3555,10 @@
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="28"/>
+      <c r="C13" s="98"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -3594,11 +3594,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="95"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
@@ -3615,10 +3615,10 @@
       <c r="A20" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="28"/>
+      <c r="C20" s="98"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
@@ -3643,11 +3643,11 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="95"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -3683,11 +3683,11 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="95"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
@@ -3734,11 +3734,11 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
+      <c r="B35" s="95"/>
+      <c r="C35" s="95"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
@@ -3766,10 +3766,10 @@
       <c r="A38" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="28"/>
+      <c r="C38" s="98"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
@@ -3786,10 +3786,10 @@
       <c r="A40" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="30"/>
+      <c r="C40" s="73"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
@@ -3824,8 +3824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDC067E-E059-49F6-9F6D-C61CC1C32937}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3835,33 +3835,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="56"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="80"/>
+      <c r="C3" s="39"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="42" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3869,7 +3869,7 @@
       <c r="A5" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="40" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3877,42 +3877,42 @@
       <c r="A6" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="56"/>
+      <c r="C6" s="31"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="56"/>
+      <c r="C7" s="31"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" s="56"/>
+      <c r="C8" s="31"/>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="61" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="79"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="38"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="101" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="80"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="39"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="37" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3920,7 +3920,7 @@
       <c r="A12" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="42" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3928,7 +3928,7 @@
       <c r="A13" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="40" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3936,35 +3936,35 @@
       <c r="A14" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="40" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="91" t="s">
+      <c r="A15" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="B15" s="91" t="s">
+      <c r="B15" s="50" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="B17" s="43"/>
+      <c r="B17" s="61"/>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="101" t="s">
         <v>113</v>
       </c>
-      <c r="B18" s="32"/>
+      <c r="B18" s="101"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="78" t="s">
+      <c r="B19" s="37" t="s">
         <v>114</v>
       </c>
     </row>
@@ -3972,7 +3972,7 @@
       <c r="A20" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="42" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3980,7 +3980,7 @@
       <c r="A21" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="40" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3988,15 +3988,15 @@
       <c r="A22" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="81" t="s">
+      <c r="B22" s="40" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="91" t="s">
+      <c r="A23" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="B23" s="91" t="s">
+      <c r="B23" s="50" t="s">
         <v>104</v>
       </c>
     </row>
@@ -4029,65 +4029,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="43" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="61" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="43"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="101" t="s">
         <v>151</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="34" t="s">
+      <c r="B2" s="101"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="E2" s="34"/>
+      <c r="E2" s="102"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="77" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="44" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="56"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="42" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="87" t="s">
+      <c r="B5" s="102"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="E5" s="88" t="s">
+      <c r="E5" s="47" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4095,14 +4095,14 @@
       <c r="A6" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="C6" s="41"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="E6" s="81" t="s">
+      <c r="E6" s="40" t="s">
         <v>145</v>
       </c>
     </row>
@@ -4110,69 +4110,69 @@
       <c r="A7" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="84"/>
-      <c r="D7" s="43" t="s">
+      <c r="C7" s="43"/>
+      <c r="D7" s="61" t="s">
         <v>150</v>
       </c>
-      <c r="E7" s="43"/>
+      <c r="E7" s="61"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="34" t="s">
+      <c r="C8" s="41"/>
+      <c r="D8" s="102" t="s">
         <v>154</v>
       </c>
-      <c r="E8" s="34"/>
+      <c r="E8" s="102"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B9" s="88" t="s">
+      <c r="B9" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="C9" s="74"/>
-      <c r="D9" s="77" t="s">
-        <v>189</v>
-      </c>
-      <c r="E9" s="85" t="s">
+      <c r="C9" s="34"/>
+      <c r="D9" s="36" t="s">
         <v>188</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="74"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="88" t="s">
+      <c r="E10" s="47" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="50" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="50" t="s">
         <v>103</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="81" t="s">
+      <c r="E11" s="40" t="s">
         <v>162</v>
       </c>
     </row>
@@ -4180,15 +4180,15 @@
       <c r="D12" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="E12" s="81" t="s">
+      <c r="E12" s="40" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="90" t="s">
-        <v>190</v>
-      </c>
-      <c r="E13" s="91" t="s">
+      <c r="D13" s="49" t="s">
+        <v>189</v>
+      </c>
+      <c r="E13" s="50" t="s">
         <v>103</v>
       </c>
     </row>
@@ -4211,8 +4211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9796394C-5BB6-4C83-86A3-B89E37E7E6DD}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4221,66 +4221,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="94"/>
+      <c r="B1" s="103"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="104" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="95"/>
+      <c r="B2" s="104"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="51" t="s">
         <v>179</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="52" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="98" t="s">
+      <c r="A4" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="54" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="98" t="s">
+      <c r="A5" s="53" t="s">
         <v>181</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="55" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="101" t="s">
+      <c r="A6" s="56" t="s">
         <v>182</v>
       </c>
-      <c r="B6" s="100" t="s">
+      <c r="B6" s="55" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="61" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="43"/>
+      <c r="B7" s="61"/>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="101" t="s">
         <v>168</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="101"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="B9" s="78" t="s">
+      <c r="B9" s="37" t="s">
         <v>169</v>
       </c>
     </row>
@@ -4288,7 +4288,7 @@
       <c r="A10" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="42" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4296,7 +4296,7 @@
       <c r="A11" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="40" t="s">
         <v>170</v>
       </c>
     </row>
@@ -4304,7 +4304,7 @@
       <c r="A12" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="40" t="s">
         <v>146</v>
       </c>
     </row>
@@ -4312,33 +4312,33 @@
       <c r="A13" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="40" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="B14" s="81"/>
+        <v>194</v>
+      </c>
+      <c r="B14" s="40"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="61" t="s">
         <v>172</v>
       </c>
-      <c r="B15" s="43"/>
+      <c r="B15" s="61"/>
     </row>
     <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="B16" s="32"/>
+      <c r="A16" s="101" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" s="101"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="37" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4346,7 +4346,7 @@
       <c r="A18" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="42" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4354,7 +4354,7 @@
       <c r="A19" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B19" s="88" t="s">
+      <c r="B19" s="47" t="s">
         <v>176</v>
       </c>
     </row>
@@ -4362,7 +4362,7 @@
       <c r="A20" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B20" s="81" t="s">
+      <c r="B20" s="40" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4370,51 +4370,51 @@
       <c r="A21" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="40" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="104" t="s">
+      <c r="A22" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="B22" s="40"/>
+    </row>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="B23" s="48"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="61" t="s">
         <v>199</v>
       </c>
-      <c r="B22" s="81"/>
-    </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="103" t="s">
-        <v>196</v>
-      </c>
-      <c r="B23" s="89"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+      <c r="B24" s="61"/>
+    </row>
+    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="58" t="s">
         <v>200</v>
       </c>
-      <c r="B24" s="43"/>
-    </row>
-    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="104" t="s">
-        <v>201</v>
-      </c>
-      <c r="B25" s="47"/>
+      <c r="B25" s="28"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="91" t="s">
-        <v>187</v>
-      </c>
-      <c r="B26" s="91" t="s">
+      <c r="A26" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="B26" s="50" t="s">
         <v>105</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>